<commit_message>
feat: Develop export attendance result to excel
</commit_message>
<xml_diff>
--- a/uef_diem_danh/ExportExcels/Attendance Result sample.xlsx
+++ b/uef_diem_danh/ExportExcels/Attendance Result sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmings\Project\Real projects\Diem_danh_nha_nuoc\real-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2027A1B-00D2-45C6-A5A3-E85A364988F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F96803A-056D-4F61-BAC3-01811185FE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,19 +86,11 @@
       <b/>
       <sz val="13"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,6 +100,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -127,15 +125,15 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -156,11 +154,17 @@
         <vertAlign val="baseline"/>
         <sz val="13"/>
         <color theme="1"/>
-        <name val="Calibri"/>
+        <name val="Arial"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -175,9 +179,9 @@
         <vertAlign val="baseline"/>
         <sz val="13"/>
         <color theme="1" tint="4.9989318521683403E-2"/>
-        <name val="Calibri"/>
+        <name val="Arial"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <fill>
@@ -200,11 +204,17 @@
         <vertAlign val="baseline"/>
         <sz val="13"/>
         <color theme="1"/>
-        <name val="Calibri"/>
+        <name val="Arial"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -219,11 +229,17 @@
         <vertAlign val="baseline"/>
         <sz val="13"/>
         <color theme="1"/>
-        <name val="Calibri"/>
+        <name val="Arial"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -238,11 +254,17 @@
         <vertAlign val="baseline"/>
         <sz val="13"/>
         <color theme="1"/>
-        <name val="Calibri"/>
+        <name val="Arial"/>
         <family val="2"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -536,53 +558,53 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H1" sqref="H1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" style="1" customWidth="1"/>
     <col min="5" max="6" width="8.88671875" style="1"/>
     <col min="7" max="7" width="7.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.44140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="14.44140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" style="1" customWidth="1"/>
     <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -593,7 +615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="16.8" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>

</xml_diff>

<commit_message>
feat: Add attendance status in export student attendance result
</commit_message>
<xml_diff>
--- a/uef_diem_danh/ExportExcels/Attendance Result sample.xlsx
+++ b/uef_diem_danh/ExportExcels/Attendance Result sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmings\Project\Real projects\Diem_danh_nha_nuoc\real-app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F96803A-056D-4F61-BAC3-01811185FE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C63B4DD-C41C-4C4C-A43F-63D737AD796F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>KẾT QUẢ ĐIỂM DANH</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Buổi: 1</t>
+  </si>
+  <si>
+    <t>Trạng thái</t>
   </si>
 </sst>
 </file>
@@ -126,9 +129,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -136,11 +136,14 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
       <font>
         <b val="0"/>
@@ -163,31 +166,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="13"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -267,6 +245,56 @@
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -281,12 +309,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A403BB5-73A3-4C8E-8F3F-88523927D748}" name="Table1" displayName="Table1" ref="A5:C6" insertRow="1" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A5:C6" xr:uid="{6A403BB5-73A3-4C8E-8F3F-88523927D748}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{70CDB739-9E54-4F14-893F-4F72C29E1230}" name="STT" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{9A47C021-2F49-4AE1-97D5-4598104B482F}" name="Họ và tên" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{A74E98BC-EF90-41BE-B44C-9E9B64A9FACD}" name="Thời gian" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A403BB5-73A3-4C8E-8F3F-88523927D748}" name="Table1" displayName="Table1" ref="A5:D6" insertRow="1" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A5:D6" xr:uid="{6A403BB5-73A3-4C8E-8F3F-88523927D748}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{70CDB739-9E54-4F14-893F-4F72C29E1230}" name="STT" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{9A47C021-2F49-4AE1-97D5-4598104B482F}" name="Họ và tên" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{A74E98BC-EF90-41BE-B44C-9E9B64A9FACD}" name="Trạng thái" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{389EA61D-EAEA-43C7-BF20-187D06233288}" name="Thời gian" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -558,7 +587,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:K1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -577,12 +606,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -605,20 +634,24 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>